<commit_message>
idk what dis is
</commit_message>
<xml_diff>
--- a/shinyapp/data/Loudoun_staffsurvey.xlsx
+++ b/shinyapp/data/Loudoun_staffsurvey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayosborne/Downloads/2022_DSPG_Loudoun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayosborne/Downloads/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1973A26-9E7B-FD4C-B129-BA9663700B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B152619-5A3A-6E42-A0B0-6E50C10A0542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="28040" windowHeight="16500" xr2:uid="{F80103EA-8F52-9546-A80A-B7A37CCE91C7}"/>
   </bookViews>
@@ -476,10 +476,13 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="86" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>